<commit_message>
add image in attendance sheet
</commit_message>
<xml_diff>
--- a/assets/excel/AttendanceSheet1.xlsx
+++ b/assets/excel/AttendanceSheet1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://700appsnet-my.sharepoint.com/personal/mohamed_sofy_700apps_net/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fci mobile project\Attendance\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2C44BDEC2040C98AC652E41EA4F5C1BC1998AE38" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35DD3171-8FEB-4B0D-ABDE-524481F6F090}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>#</t>
   </si>
@@ -67,16 +66,48 @@
   </si>
   <si>
     <t>mohsen</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>https://img.freepik.com/free-photo/handsome-young-man-with-arms-crossed-white-background_23-2148222620.jpg</t>
+  </si>
+  <si>
+    <t>https://img.freepik.com/free-photo/handsome-confident-smiling-man-with-hands-crossed-chest_176420-18743.jpg</t>
+  </si>
+  <si>
+    <t>https://img.freepik.com/free-photo/attractive-mixed-race-male-with-positive-smile-shows-white-teeth-keeps-hands-stomach-being-high-spirit-wears-white-shirt-rejoices-positive-moments-life-people-emotions-concept_273609-15527.jpg</t>
+  </si>
+  <si>
+    <t>https://img.freepik.com/free-photo/confident-handsome-guy-posing-against-white-wall_176420-32936.jpg</t>
+  </si>
+  <si>
+    <t>https://img.freepik.com/free-photo/fashionable-stylish-man-with-dark-eyes-casual-clothes-looking-aside-with-placid-thoughtful-look-pensive-guy-with-puzzled-expression-thinking-about-something-building-plans_176420-10331.jpg</t>
+  </si>
+  <si>
+    <t>https://img.freepik.com/free-photo/thoughtful-concerned-man-thinking-trying-find-solution_176420-19574.jpg</t>
+  </si>
+  <si>
+    <t>https://img.freepik.com/free-photo/serious-thoughtful-man-squinting-skeptical-thinking-as-making-choice_176420-19020.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,14 +130,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -384,16 +418,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E1" sqref="E1:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,8 +440,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -420,8 +457,11 @@
       <c r="D2" s="1">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -434,8 +474,11 @@
       <c r="D3" s="1">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -448,8 +491,11 @@
       <c r="D4" s="1">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -462,8 +508,11 @@
       <c r="D5" s="1">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -476,8 +525,11 @@
       <c r="D6" s="1">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -490,8 +542,11 @@
       <c r="D7" s="1">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -504,8 +559,11 @@
       <c r="D8" s="1">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -518,8 +576,11 @@
       <c r="D9" s="1">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -532,8 +593,11 @@
       <c r="D10" s="1">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -546,8 +610,16 @@
       <c r="D11" s="1">
         <v>0.41666666666666669</v>
       </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="E7" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>